<commit_message>
ajustes según nuevos criterios
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado09/guion05/Escaleta_CS_09_05_CO.xlsx
+++ b/fuentes/contenidos/grado09/guion05/Escaleta_CS_09_05_CO.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="162">
   <si>
     <t>Asignatura</t>
   </si>
@@ -466,9 +466,6 @@
     <t>CS_09_05_CO</t>
   </si>
   <si>
-    <t>Las causas de la Segunda Guerra Mundial</t>
-  </si>
-  <si>
     <t>Actividad que repasa las causas de la Segunda Guerra Mundial</t>
   </si>
   <si>
@@ -503,6 +500,12 @@
   </si>
   <si>
     <t>m1c</t>
+  </si>
+  <si>
+    <t>Actividad que repasa los orígenes de la Segunda Guerra Mundial</t>
+  </si>
+  <si>
+    <t>los orígenes de la Segunda Guerra Mundial</t>
   </si>
 </sst>
 </file>
@@ -822,7 +825,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
@@ -946,6 +949,9 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1219,7 +1225,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1229,8 +1235,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H31" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="L40" sqref="L40"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1317,7 +1323,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:20" s="62" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" s="62" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="58" t="s">
         <v>66</v>
       </c>
@@ -1332,23 +1338,23 @@
       </c>
       <c r="E2" s="58"/>
       <c r="F2" s="58"/>
-      <c r="G2" s="62" t="s">
-        <v>148</v>
+      <c r="G2" s="74" t="s">
+        <v>161</v>
       </c>
       <c r="H2" s="62">
         <v>1</v>
       </c>
-      <c r="I2" s="62" t="s">
+      <c r="I2" s="64" t="s">
         <v>20</v>
       </c>
       <c r="J2" s="73" t="s">
-        <v>149</v>
+        <v>160</v>
       </c>
       <c r="K2" s="63" t="s">
         <v>69</v>
       </c>
       <c r="L2" s="64" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="M2" s="67"/>
       <c r="N2" s="64"/>
@@ -1424,7 +1430,7 @@
       <c r="E4" s="51"/>
       <c r="F4" s="52"/>
       <c r="G4" s="65" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H4" s="60">
         <v>3</v>
@@ -1433,7 +1439,7 @@
         <v>20</v>
       </c>
       <c r="J4" s="66" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="K4" s="51" t="s">
         <v>69</v>
@@ -1515,7 +1521,7 @@
       <c r="E6" s="54"/>
       <c r="F6" s="55"/>
       <c r="G6" s="53" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H6" s="56">
         <v>5</v>
@@ -1524,7 +1530,7 @@
         <v>19</v>
       </c>
       <c r="J6" s="57" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K6" s="51" t="s">
         <v>69</v>
@@ -1654,15 +1660,15 @@
         <v>8</v>
       </c>
       <c r="I9" s="56" t="s">
+        <v>153</v>
+      </c>
+      <c r="J9" s="57" t="s">
         <v>154</v>
-      </c>
-      <c r="J9" s="57" t="s">
-        <v>155</v>
       </c>
       <c r="K9" s="51"/>
       <c r="L9" s="58"/>
       <c r="M9" s="58" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="N9" s="69"/>
       <c r="O9" s="60"/>
@@ -2019,7 +2025,7 @@
       </c>
       <c r="F17" s="55"/>
       <c r="G17" s="53" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H17" s="56">
         <v>140</v>
@@ -2028,7 +2034,7 @@
         <v>19</v>
       </c>
       <c r="J17" s="57" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K17" s="54"/>
       <c r="L17" s="58"/>
@@ -2211,14 +2217,14 @@
       <c r="E21" s="54"/>
       <c r="F21" s="55"/>
       <c r="G21" s="53" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H21" s="56">
         <v>180</v>
       </c>
       <c r="I21" s="56"/>
       <c r="J21" s="57" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="K21" s="54" t="s">
         <v>69</v>

</xml_diff>